<commit_message>
Data Drive the script1
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\B93 Selenium\AFW\pos-afw\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C15791-5EDA-41D4-AF25-AC8F92FC5D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2F535F-5A30-4197-869E-6EF6FC72E108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,9 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Jai Ganesh</t>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>pointofsale</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Passsword</t>
   </si>
 </sst>
 </file>
@@ -345,17 +354,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automation Script for invalid login
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\B93 Selenium\AFW\pos-afw\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2F535F-5A30-4197-869E-6EF6FC72E108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1B99C4-04A1-4D07-8450-659660B79523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>admin</t>
   </si>
@@ -37,6 +38,21 @@
   </si>
   <si>
     <t>Passsword</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ErrMsg</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>Invalid username and/or password.</t>
   </si>
 </sst>
 </file>
@@ -356,7 +372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -384,4 +400,46 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DB43D3-9944-4361-A854-B522D6351709}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>